<commit_message>
Just changed some of the punctuation/capitalization in the doc
</commit_message>
<xml_diff>
--- a/DevelopmentSchedule.xlsx
+++ b/DevelopmentSchedule.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdols\Documents\CSC323\Robots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariabolt/Desktop/team1se/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B14290A-8C77-4ADD-B6D4-2C8E0F70874A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,11 +35,20 @@
     <t>Note: the customer may tell you you did something wrong and have to change it!</t>
   </si>
   <si>
-    <t>Note: Don't spend hours on quality art. You aren't judged on the prettiness of the art. (or sound). Just make it look kind of like it is supposed too</t>
+    <t>Robot RPG Development Schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Groups will have to talk to the customer to clarify points. </t>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>Task</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">the game will have two types of movement. An overworld where the player will move around and the fix it phase, where the player will have to fix robots, avoiding obstacles along the way. the player will be able, upon colliding with an robot in the overworld, be brought to a "place" to fix a robot. </t>
+      <t xml:space="preserve">The game will have two types of movement. An overworld where the player will move around, and the fix it phase, where the player will have to fix robots, avoiding obstacles along the way. The player will be able, upon colliding with a robot in the overworld, be brought to a "place" to fix a robot. </t>
     </r>
     <r>
       <rPr>
@@ -46,56 +60,47 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">The robot will be moving around in a pre-defined way and the player will have to be careful to avoid being injured while attempting to fix it. </t>
+      <t xml:space="preserve">The robot will be moving around in a pre-defined way, and the player will have to be careful to avoid being injured while attempting to fix it. </t>
     </r>
   </si>
   <si>
-    <t>To fix a robot, the player throws replacement parts at it. Replacement parts are thrown in the way the player last moved (or the way the player last tried to move). multiple robots can be on the same board at once. No character can occupy the same cell as another character</t>
-  </si>
-  <si>
-    <t>the robot and player will be on 8x8 grid in the fix it mode. They player/robots "snap" to the center of a new square on the grid when they move.  There will be different kinds of robots and each will be unique (in how they damage the player, how they move)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the player will be able to walk in an overworld consisting of villages, people, and broken robots. Between the villages are spaces where robots exist. </t>
-  </si>
-  <si>
-    <t>The player will be able to pickup new types of ways to fix robots when the player successfully fixes a robot or in chests in the overworld. The player will be able to select 4 different ways of fixing robots per "fix it" phase (this should be in a menu that can be brought up in the overworld)</t>
-  </si>
-  <si>
-    <t>the player will be able to "talk" to people -&gt; that is, text should appear when the player presses a certain key. The key should be "scrollable", meaning that for a long text box, part of the text will initially apear; then, after the players presses a key, the next part of the text will appear until all the text has appeared.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">the robots will walk along set paths in the overworld. They will appear and disappear at points. If the player gets "to close" to a robot, the robot will attempt to chase the player. They player should be able to jump in the overworld, walk and run. They player can jump over a chasing robot. </t>
-  </si>
-  <si>
-    <t>at the conclusion of a fix it phase, the player is taken back to the overworld, where the locations of all NPCs (robots, villagers) should be the same as when the player was brought to the fix it phase</t>
-  </si>
-  <si>
-    <t>create a simple story for the game. A story can be given by the client if one is not thought of by the programmers. When the player fixes the "boss" robot, they win. The boss robot should be unique.</t>
-  </si>
-  <si>
-    <t>create a menu for the game.  There should be at least 5 types fo robots, 10 different ways to fix robots, five towns to journey too.</t>
-  </si>
-  <si>
-    <t>Robot RPG Development Schedule</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: Groups will have to talk to the customer to clarify points. </t>
-  </si>
-  <si>
-    <t>Note: the customer expects it will work! A story that does not work is not complete</t>
-  </si>
-  <si>
-    <t>Iteration</t>
-  </si>
-  <si>
-    <t>Task</t>
+    <t>To fix a robot, the player throws replacement parts at it. Replacement parts are thrown in the way the player last moved (or the way the player last tried to move). Multiple robots can be on the same board at once. No character can occupy the same cell as another character.</t>
+  </si>
+  <si>
+    <t>The robot and player will be on 8x8 grid in the fix it mode. They player/robots "snap" to the center of a new square on the grid when they move.  There will be different kinds of robots and each will be unique (in how they damage the player, how they move).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The player will be able to walk in an overworld consisting of villages, people, and broken robots. Between the villages are spaces where robots exist. </t>
+  </si>
+  <si>
+    <t>The player will be able to pickup new types of ways to fix robots when they successfully fix a robot or in chests in the overworld. The player will be able to select 4 different ways of fixing robots per "fix it" phase (this should be in a menu that can be brought up in the overworld).</t>
+  </si>
+  <si>
+    <t>The player will be able to "talk" to people -&gt; that is, text should appear when the player presses a certain key. The key should be "scrollable", meaning that for a long text box, part of the text will initially apear; then, after the players presses a key, the next part of the text will appear until all the text has appeared.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The robots will walk along set paths in the overworld. They will appear and disappear at points. If the player gets "to close" to a robot, the robot will attempt to chase the player. They player should be able to jump, walk and run in the overworld. They player can jump over a chasing robot. </t>
+  </si>
+  <si>
+    <t>At the conclusion of a fix it phase, the player is taken back to the overworld, where the locations of all NPCs (robots, villagers) should be the same as when the player was brought to the fix it phase.</t>
+  </si>
+  <si>
+    <t>Create a simple story for the game. A story can be given by the client if one is not thought of by the programmers. When the player fixes the "boss" robot, they win. The boss robot should be unique.</t>
+  </si>
+  <si>
+    <t>Create a menu for the game.  There should be at least 5 types fo robots, 10 different ways to fix robots, and five towns to journey to.</t>
+  </si>
+  <si>
+    <t>Note: Don't spend hours on quality art. You aren't judged on the prettiness of the art (or sound). Just make it look kind of like it is supposed too.</t>
+  </si>
+  <si>
+    <t>Note: the customer expects it will work! A story that does not work is not complete.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,42 +189,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -227,23 +232,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -256,6 +261,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -268,43 +285,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -586,188 +591,188 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.83984375" customWidth="1"/>
-    <col min="3" max="3" width="28.734375" customWidth="1"/>
-    <col min="4" max="4" width="25.26171875" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" ht="105.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" ht="105.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="9">
+      <c r="B7" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="63.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B8" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:10" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="63.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9">
-        <v>1</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="B10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>2</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>2</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" ht="64.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>3</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" ht="53.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="11">
-        <v>2</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="1:10" ht="62.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="11">
-        <v>2</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="11">
-        <v>2</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" ht="64.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="12">
-        <v>3</v>
-      </c>
       <c r="B13" s="13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="12">
+    <row r="14" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>3</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="12">
+    <row r="15" spans="1:10" ht="49.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>3</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:10" ht="47.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="12">
+    <row r="16" spans="1:10" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>3</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -775,11 +780,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B14:E14"/>
@@ -791,6 +791,11 @@
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>